<commit_message>
Update para executar com o BD_CODIGOS e manter a ordenação correta dos labels
</commit_message>
<xml_diff>
--- a/Sintaxe_Exemplo.xlsx
+++ b/Sintaxe_Exemplo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROJETOS\Processamento-Estatistico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288CE3F7-F88F-43FC-8CEF-A4F52351E5C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40180706-A58D-49F5-9108-D55ADEB23E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,7 +61,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Informar as colunas (bandeiras) que representa as colunas da tabela, separados por ", " (virgula espaço).</t>
+Informar as colunas (bandeiras) que representa as colunas da tabela, separados por ", " (virgula e um espaço).</t>
         </r>
       </text>
     </comment>
@@ -85,7 +85,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Informar o nome do cabeçalho desejado para as colunas da bandeira. Coloque o cabeçalho separado por ", " (virgula espaço).</t>
+Informar o nome do cabeçalho desejado para as colunas da bandeira. Coloque o cabeçalho separado por ", " (virgula e um espaço).</t>
         </r>
       </text>
     </comment>
@@ -109,7 +109,9 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Nome da variável que representa a linha da tabela.</t>
+Nome da variável que representa a linha da tabela. 
+Obs.: quando a variável que representa a linha for de uma tabela MULTIPLA é necessário colocar um nome diferente dos Valores_Agrup.
+Exemplo: Variáveis REC_1, REC_2, REC_3 que referem a uma MULTIPLA, o nome da variável que representa a linha da tabela poderá ser REC, ou seja, diferente dos nomes das variáveis que serão preenchidas no campo: “Valores_Agrup”.</t>
         </r>
       </text>
     </comment>
@@ -133,7 +135,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-A tabela deverá contabilizar os casos de `NS/NR` Escreva SIM ou NAO (em maiuscula e sem acento)? </t>
+A tabela deverá contabilizar os casos de `NS/NR`? Escreva SIM ou NAO (em maiuscula e sem acento). </t>
         </r>
       </text>
     </comment>
@@ -157,7 +159,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Somente quando a variável que representará as linhas for do TipoTabela IPA_10, informar os valores a serem considerados para o BTB separados por vírgula e espaço (, ).</t>
+Somente quando a variável que representará as linhas for do TipoTabela IPA_10 ou IPA_5, informar os valores a serem considerados para o BTB separados por ", " (virgula e um espaço).</t>
         </r>
       </text>
     </comment>
@@ -181,7 +183,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Somente quando a variável que representará as linhas for do TipoTabela IPA_10, informar os valores a serem considerados para o TTB separados por vírgula e espaço (, ).</t>
+Somente quando a variável que representará as linhas for do TipoTabela IPA_10 ou IPA_5, informar os valores a serem considerados para o TTB separados por ", " (virgula e um espaço).</t>
         </r>
       </text>
     </comment>
@@ -205,7 +207,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Informar somente quando a variável na linha for IPA_5 (deverá informar os nomes das categorias do IPA_5 em ordem, da pior categoria até a melhor) ou MULTIPLA (deverá informar o nome das colunas que descrevem a variável múltipla. Coloque  separdo por ", " (virgula espaço)</t>
+Informar somente quando a variável na linha for MULTIPLA (deverá informar o nome das colunas que descrevem a variável múltipla. Coloque  separdo por ", " (virgula e um espaço).</t>
         </r>
       </text>
     </comment>
@@ -289,7 +291,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Rayner Santos:</t>
         </r>
@@ -298,7 +300,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Informar o título da tabela</t>
@@ -310,7 +312,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
   <si>
     <t>TipoTabela</t>
   </si>
@@ -327,46 +329,91 @@
     <t>NPS</t>
   </si>
   <si>
+    <t>NPS_C</t>
+  </si>
+  <si>
+    <t>POND</t>
+  </si>
+  <si>
+    <t>C_26</t>
+  </si>
+  <si>
+    <t>SIMPLES</t>
+  </si>
+  <si>
+    <t>VREG</t>
+  </si>
+  <si>
+    <t>IPA_5</t>
+  </si>
+  <si>
+    <t>VCH_C</t>
+  </si>
+  <si>
+    <t>MULTIPLA</t>
+  </si>
+  <si>
+    <t>Contabiliza_NS/NR</t>
+  </si>
+  <si>
+    <t>BTB</t>
+  </si>
+  <si>
+    <t>TTB</t>
+  </si>
+  <si>
+    <t>NAO</t>
+  </si>
+  <si>
+    <t>IPA_10</t>
+  </si>
+  <si>
+    <t>REC</t>
+  </si>
+  <si>
+    <t>Fecha_100</t>
+  </si>
+  <si>
+    <t>Bandeiras</t>
+  </si>
+  <si>
+    <t>ID_EMP</t>
+  </si>
+  <si>
+    <t>Var_ID</t>
+  </si>
+  <si>
+    <t>Cabecalho</t>
+  </si>
+  <si>
+    <t>Titulo</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>Título 1</t>
+  </si>
+  <si>
+    <t>Título 2</t>
+  </si>
+  <si>
+    <t>Título 3</t>
+  </si>
+  <si>
+    <t>Título 4</t>
+  </si>
+  <si>
+    <t>Título 5</t>
+  </si>
+  <si>
     <t>ONDA, EMP_G, VAR_G, GC_G, ME_G, ESP_G, PJ_G, PF_G</t>
   </si>
   <si>
-    <t>NPS_C</t>
-  </si>
-  <si>
-    <t>POND</t>
-  </si>
-  <si>
-    <t>C_26</t>
-  </si>
-  <si>
-    <t>SIMPLES</t>
-  </si>
-  <si>
-    <t>VREG</t>
-  </si>
-  <si>
-    <t>IPA_5</t>
-  </si>
-  <si>
-    <t>VCH_C</t>
-  </si>
-  <si>
-    <t>MULTIPLA</t>
-  </si>
-  <si>
-    <t>Contabiliza_NS/NR</t>
-  </si>
-  <si>
-    <t>BTB</t>
-  </si>
-  <si>
-    <t>TTB</t>
-  </si>
-  <si>
-    <t>NAO</t>
-  </si>
-  <si>
-    <t>IPA_10</t>
+    <t>ONDA, Empreendedores, Varejo, GC, ME, Especiais, Pessoa Jurídica, Pessoa Física</t>
+  </si>
+  <si>
+    <t>REC_1, REC_2, REC_3</t>
   </si>
   <si>
     <t>1, 2, 3, 4, 5</t>
@@ -375,59 +422,17 @@
     <t>8, 9, 10</t>
   </si>
   <si>
-    <t>REC_1, REC_2, REC_3</t>
-  </si>
-  <si>
-    <t>REC</t>
-  </si>
-  <si>
-    <t>Com certeza deixaria de trabalhar, Provavelmente deixaria de trabalhar, Não sei se vou continuar ou não, Provavelmente continuaria trabalhando, Com certeza continuaria trabalhando</t>
-  </si>
-  <si>
-    <t>Fecha_100</t>
-  </si>
-  <si>
-    <t>Bandeiras</t>
-  </si>
-  <si>
-    <t>ID_EMP</t>
-  </si>
-  <si>
-    <t>Var_ID</t>
-  </si>
-  <si>
-    <t>Cabecalho</t>
-  </si>
-  <si>
-    <t>Titulo</t>
-  </si>
-  <si>
-    <t>ONDA, Empreendedores, Varejo, GC, ME, Especiais, Pessoa Jurídica, Pessoa Física</t>
-  </si>
-  <si>
-    <t>.</t>
-  </si>
-  <si>
-    <t>Título 1</t>
-  </si>
-  <si>
-    <t>Título 2</t>
-  </si>
-  <si>
-    <t>Título 3</t>
-  </si>
-  <si>
-    <t>Título 4</t>
-  </si>
-  <si>
-    <t>Título 5</t>
+    <t>1, 2</t>
+  </si>
+  <si>
+    <t>4, 5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -461,19 +466,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -815,23 +807,23 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.77734375" customWidth="1"/>
+    <col min="6" max="6" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5546875" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.88671875" customWidth="1"/>
+    <col min="12" max="12" width="16.33203125" customWidth="1"/>
     <col min="13" max="13" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -840,67 +832,67 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -908,131 +900,133 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="K4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="E6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>